<commit_message>
Napisano polowe obliczen na sprawko
</commit_message>
<xml_diff>
--- a/FIZ2/Halla.xlsx
+++ b/FIZ2/Halla.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kamil\Desktop\Stary Folder\studia\fizyka\Fizyka_2\laby\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kamil\Desktop\Stary Folder\studia_git\FIZ2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AFCF23-AD9F-4B25-BAB6-DA6B2779E60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FD1598-101F-4530-A56E-17247E67515B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22106E2D-535D-4D61-8847-61EECC787C3F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
   <si>
     <t>B[mT]</t>
   </si>
@@ -117,6 +117,54 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>spr</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>AD2</t>
+  </si>
+  <si>
+    <t>AD4</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>AD5</t>
+  </si>
+  <si>
+    <t>uc(Uh)</t>
+  </si>
+  <si>
+    <t>u(a)</t>
+  </si>
+  <si>
+    <t>u(b)</t>
+  </si>
+  <si>
+    <t>AD6</t>
+  </si>
+  <si>
+    <t>uc,r(Uh)</t>
+  </si>
+  <si>
+    <t>Uh</t>
+  </si>
+  <si>
+    <t>AD7</t>
+  </si>
+  <si>
+    <t>U(Uh)</t>
   </si>
 </sst>
 </file>
@@ -124,7 +172,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -346,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -364,7 +412,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -383,9 +433,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Pakiet Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -423,7 +473,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Pakiet Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -529,7 +579,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Pakiet Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -671,7 +721,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -679,19 +729,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A447AA0A-D447-4B02-AC14-94CF8529AAB0}">
-  <dimension ref="C4:V37"/>
+  <dimension ref="C1:DD85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="C15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.5703125" customWidth="1"/>
+    <col min="24" max="108" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:108" x14ac:dyDescent="0.25">
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+    </row>
+    <row r="2" spans="3:108" x14ac:dyDescent="0.25">
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+    </row>
+    <row r="3" spans="3:108" x14ac:dyDescent="0.25">
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="18"/>
+    </row>
+    <row r="4" spans="3:108" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T4" t="s">
         <v>9</v>
       </c>
@@ -701,8 +765,266 @@
       <c r="V4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="W4" t="s">
+        <v>27</v>
+      </c>
+      <c r="X4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="9">
+        <v>10</v>
+      </c>
+      <c r="AA4" s="9">
+        <v>20</v>
+      </c>
+      <c r="AB4" s="9">
+        <v>30</v>
+      </c>
+      <c r="AC4" s="9">
+        <v>40</v>
+      </c>
+      <c r="AD4" s="9">
+        <v>50</v>
+      </c>
+      <c r="AE4" s="9">
+        <v>60</v>
+      </c>
+      <c r="AF4" s="9">
+        <v>70</v>
+      </c>
+      <c r="AG4" s="9">
+        <v>80</v>
+      </c>
+      <c r="AH4" s="9">
+        <v>90</v>
+      </c>
+      <c r="AI4" s="9">
+        <v>100</v>
+      </c>
+      <c r="AJ4" s="9">
+        <v>110</v>
+      </c>
+      <c r="AK4" s="9">
+        <v>120</v>
+      </c>
+      <c r="AL4" s="9">
+        <v>130</v>
+      </c>
+      <c r="AM4" s="9">
+        <v>140</v>
+      </c>
+      <c r="AN4" s="9">
+        <v>150</v>
+      </c>
+      <c r="AO4" s="9">
+        <v>160</v>
+      </c>
+      <c r="AP4" s="9">
+        <v>170</v>
+      </c>
+      <c r="AQ4" s="9">
+        <v>180</v>
+      </c>
+      <c r="AR4" s="9">
+        <v>190</v>
+      </c>
+      <c r="AS4" s="11">
+        <v>200</v>
+      </c>
+      <c r="AT4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="4">
+        <v>-10</v>
+      </c>
+      <c r="AV4" s="4">
+        <v>-20</v>
+      </c>
+      <c r="AW4" s="4">
+        <v>-30</v>
+      </c>
+      <c r="AX4" s="4">
+        <v>-40</v>
+      </c>
+      <c r="AY4" s="4">
+        <v>-50</v>
+      </c>
+      <c r="AZ4" s="4">
+        <v>-60</v>
+      </c>
+      <c r="BA4" s="4">
+        <v>-70</v>
+      </c>
+      <c r="BB4" s="4">
+        <v>-80</v>
+      </c>
+      <c r="BC4" s="4">
+        <v>-90</v>
+      </c>
+      <c r="BD4" s="4">
+        <v>-100</v>
+      </c>
+      <c r="BE4" s="4">
+        <v>-110</v>
+      </c>
+      <c r="BF4" s="4">
+        <v>-120</v>
+      </c>
+      <c r="BG4" s="4">
+        <v>-130</v>
+      </c>
+      <c r="BH4" s="4">
+        <v>-140</v>
+      </c>
+      <c r="BI4" s="4">
+        <v>-150</v>
+      </c>
+      <c r="BJ4" s="4">
+        <v>-160</v>
+      </c>
+      <c r="BK4" s="4">
+        <v>-170</v>
+      </c>
+      <c r="BL4" s="4">
+        <v>-180</v>
+      </c>
+      <c r="BM4" s="4">
+        <v>-190</v>
+      </c>
+      <c r="BN4" s="12">
+        <v>-200</v>
+      </c>
+      <c r="BO4" s="8">
+        <v>0</v>
+      </c>
+      <c r="BP4" s="8">
+        <v>10</v>
+      </c>
+      <c r="BQ4" s="8">
+        <v>20</v>
+      </c>
+      <c r="BR4" s="8">
+        <v>30</v>
+      </c>
+      <c r="BS4" s="8">
+        <v>40</v>
+      </c>
+      <c r="BT4" s="8">
+        <v>50</v>
+      </c>
+      <c r="BU4" s="8">
+        <v>60</v>
+      </c>
+      <c r="BV4" s="8">
+        <v>70</v>
+      </c>
+      <c r="BW4" s="8">
+        <v>80</v>
+      </c>
+      <c r="BX4" s="8">
+        <v>90</v>
+      </c>
+      <c r="BY4" s="8">
+        <v>100</v>
+      </c>
+      <c r="BZ4" s="8">
+        <v>110</v>
+      </c>
+      <c r="CA4" s="8">
+        <v>120</v>
+      </c>
+      <c r="CB4" s="8">
+        <v>130</v>
+      </c>
+      <c r="CC4" s="8">
+        <v>140</v>
+      </c>
+      <c r="CD4" s="8">
+        <v>150</v>
+      </c>
+      <c r="CE4" s="8">
+        <v>160</v>
+      </c>
+      <c r="CF4" s="8">
+        <v>170</v>
+      </c>
+      <c r="CG4" s="8">
+        <v>180</v>
+      </c>
+      <c r="CH4" s="8">
+        <v>190</v>
+      </c>
+      <c r="CI4" s="14">
+        <v>200</v>
+      </c>
+      <c r="CJ4" s="4">
+        <v>0</v>
+      </c>
+      <c r="CK4" s="4">
+        <v>-10</v>
+      </c>
+      <c r="CL4" s="4">
+        <v>-20</v>
+      </c>
+      <c r="CM4" s="4">
+        <v>-30</v>
+      </c>
+      <c r="CN4" s="4">
+        <v>-40</v>
+      </c>
+      <c r="CO4" s="4">
+        <v>-50</v>
+      </c>
+      <c r="CP4" s="4">
+        <v>-60</v>
+      </c>
+      <c r="CQ4" s="4">
+        <v>-70</v>
+      </c>
+      <c r="CR4" s="4">
+        <v>-80</v>
+      </c>
+      <c r="CS4" s="4">
+        <v>-90</v>
+      </c>
+      <c r="CT4" s="4">
+        <v>-100</v>
+      </c>
+      <c r="CU4" s="4">
+        <v>-110</v>
+      </c>
+      <c r="CV4" s="4">
+        <v>-120</v>
+      </c>
+      <c r="CW4" s="4">
+        <v>-130</v>
+      </c>
+      <c r="CX4" s="4">
+        <v>-140</v>
+      </c>
+      <c r="CY4" s="4">
+        <v>-150</v>
+      </c>
+      <c r="CZ4" s="4">
+        <v>-160</v>
+      </c>
+      <c r="DA4" s="4">
+        <v>-170</v>
+      </c>
+      <c r="DB4" s="4">
+        <v>-180</v>
+      </c>
+      <c r="DC4" s="4">
+        <v>-190</v>
+      </c>
+      <c r="DD4" s="12">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="5" spans="3:108" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
@@ -736,8 +1058,266 @@
       <c r="V5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="W5" t="s">
+        <v>28</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="Z5">
+        <v>2.1</v>
+      </c>
+      <c r="AA5" s="4">
+        <v>4</v>
+      </c>
+      <c r="AB5" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="AC5" s="4">
+        <v>7.8</v>
+      </c>
+      <c r="AD5" s="4">
+        <v>9.6</v>
+      </c>
+      <c r="AE5" s="4">
+        <v>11.5</v>
+      </c>
+      <c r="AF5" s="4">
+        <v>13.4</v>
+      </c>
+      <c r="AG5" s="4">
+        <v>15.1</v>
+      </c>
+      <c r="AH5" s="4">
+        <v>17</v>
+      </c>
+      <c r="AI5" s="4">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="AJ5" s="4">
+        <v>20.5</v>
+      </c>
+      <c r="AK5" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="AL5" s="4">
+        <v>24</v>
+      </c>
+      <c r="AM5" s="4">
+        <v>25.8</v>
+      </c>
+      <c r="AN5" s="4">
+        <v>27.6</v>
+      </c>
+      <c r="AO5" s="4">
+        <v>29.3</v>
+      </c>
+      <c r="AP5" s="4">
+        <v>31</v>
+      </c>
+      <c r="AQ5" s="4">
+        <v>32.6</v>
+      </c>
+      <c r="AR5" s="4">
+        <v>34.4</v>
+      </c>
+      <c r="AS5" s="12">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="AT5" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="AU5" s="4">
+        <v>-1.9</v>
+      </c>
+      <c r="AV5" s="4">
+        <v>-3.8</v>
+      </c>
+      <c r="AW5" s="4">
+        <v>-5</v>
+      </c>
+      <c r="AX5" s="4">
+        <v>-7.4</v>
+      </c>
+      <c r="AY5" s="4">
+        <v>-9.1999999999999993</v>
+      </c>
+      <c r="AZ5" s="4">
+        <v>-11.1</v>
+      </c>
+      <c r="BA5" s="4">
+        <v>-13</v>
+      </c>
+      <c r="BB5" s="4">
+        <v>-14.8</v>
+      </c>
+      <c r="BC5" s="4">
+        <v>-16.600000000000001</v>
+      </c>
+      <c r="BD5" s="4">
+        <v>-18.5</v>
+      </c>
+      <c r="BE5" s="4">
+        <v>-20.2</v>
+      </c>
+      <c r="BF5" s="4">
+        <v>-21.9</v>
+      </c>
+      <c r="BG5" s="4">
+        <v>-23.8</v>
+      </c>
+      <c r="BH5" s="4">
+        <v>-25.4</v>
+      </c>
+      <c r="BI5" s="4">
+        <v>-27.2</v>
+      </c>
+      <c r="BJ5" s="4">
+        <v>-28.9</v>
+      </c>
+      <c r="BK5" s="4">
+        <v>-30.8</v>
+      </c>
+      <c r="BL5" s="4">
+        <v>-32.4</v>
+      </c>
+      <c r="BM5" s="4">
+        <v>-34</v>
+      </c>
+      <c r="BN5" s="12">
+        <v>-36</v>
+      </c>
+      <c r="BO5" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="BP5" s="4">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="BQ5" s="4">
+        <v>-3.2</v>
+      </c>
+      <c r="BR5" s="4">
+        <v>-5.2</v>
+      </c>
+      <c r="BS5" s="4">
+        <v>-7.3</v>
+      </c>
+      <c r="BT5" s="4">
+        <v>-9.4</v>
+      </c>
+      <c r="BU5" s="4">
+        <v>-11.6</v>
+      </c>
+      <c r="BV5" s="4">
+        <v>-13.6</v>
+      </c>
+      <c r="BW5" s="4">
+        <v>-15.5</v>
+      </c>
+      <c r="BX5" s="4">
+        <v>-17.399999999999999</v>
+      </c>
+      <c r="BY5" s="4">
+        <v>-19.399999999999999</v>
+      </c>
+      <c r="BZ5" s="4">
+        <v>-21.6</v>
+      </c>
+      <c r="CA5" s="4">
+        <v>-23.6</v>
+      </c>
+      <c r="CB5" s="4">
+        <v>-25.3</v>
+      </c>
+      <c r="CC5" s="4">
+        <v>-27.4</v>
+      </c>
+      <c r="CD5" s="4">
+        <v>-29.9</v>
+      </c>
+      <c r="CE5" s="4">
+        <v>-31.3</v>
+      </c>
+      <c r="CF5" s="4">
+        <v>-33.299999999999997</v>
+      </c>
+      <c r="CG5" s="4">
+        <v>-35</v>
+      </c>
+      <c r="CH5" s="4">
+        <v>-36.799999999999997</v>
+      </c>
+      <c r="CI5" s="12">
+        <v>-38.700000000000003</v>
+      </c>
+      <c r="CJ5" s="4">
+        <v>0</v>
+      </c>
+      <c r="CK5" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="CL5" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="CM5" s="4">
+        <v>6.3</v>
+      </c>
+      <c r="CN5" s="4">
+        <v>8.4</v>
+      </c>
+      <c r="CO5" s="4">
+        <v>10.6</v>
+      </c>
+      <c r="CP5" s="4">
+        <v>12.6</v>
+      </c>
+      <c r="CQ5" s="4">
+        <v>14.5</v>
+      </c>
+      <c r="CR5" s="4">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="CS5" s="4">
+        <v>18.5</v>
+      </c>
+      <c r="CT5" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="CU5" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="CV5" s="4">
+        <v>24.4</v>
+      </c>
+      <c r="CW5" s="4">
+        <v>26.4</v>
+      </c>
+      <c r="CX5" s="4">
+        <v>28.3</v>
+      </c>
+      <c r="CY5" s="4">
+        <v>30.2</v>
+      </c>
+      <c r="CZ5" s="4">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="DA5" s="4">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="DB5" s="4">
+        <v>36</v>
+      </c>
+      <c r="DC5" s="4">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="DD5" s="12">
+        <v>39.6</v>
+      </c>
+    </row>
+    <row r="6" spans="3:108" x14ac:dyDescent="0.25">
       <c r="G6" s="5" t="s">
         <v>4</v>
       </c>
@@ -783,8 +1363,10 @@
       <c r="V6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="18"/>
+    </row>
+    <row r="7" spans="3:108" x14ac:dyDescent="0.25">
       <c r="G7" s="9" t="s">
         <v>0</v>
       </c>
@@ -830,8 +1412,10 @@
       <c r="V7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="18"/>
+    </row>
+    <row r="8" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C8">
         <f>G8*H8</f>
         <v>0</v>
@@ -893,8 +1477,10 @@
       <c r="V8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="18"/>
+    </row>
+    <row r="9" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C9">
         <f t="shared" ref="C9:C28" si="0">G9*H9</f>
         <v>21</v>
@@ -956,8 +1542,10 @@
       <c r="V9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="18"/>
+    </row>
+    <row r="10" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C10">
         <f t="shared" si="0"/>
         <v>80</v>
@@ -1010,8 +1598,10 @@
       <c r="R10" s="10">
         <v>-1.462</v>
       </c>
-    </row>
-    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="18"/>
+    </row>
+    <row r="11" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C11">
         <f t="shared" si="0"/>
         <v>177</v>
@@ -1064,8 +1654,10 @@
       <c r="R11" s="10">
         <v>-1.462</v>
       </c>
-    </row>
-    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="18"/>
+    </row>
+    <row r="12" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C12">
         <f t="shared" si="0"/>
         <v>312</v>
@@ -1118,8 +1710,10 @@
       <c r="R12" s="10">
         <v>-1.462</v>
       </c>
-    </row>
-    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="Y12" s="18"/>
+      <c r="Z12" s="18"/>
+    </row>
+    <row r="13" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C13">
         <f t="shared" si="0"/>
         <v>480</v>
@@ -1172,8 +1766,10 @@
       <c r="R13" s="10">
         <v>-1.4630000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="18"/>
+    </row>
+    <row r="14" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C14">
         <f t="shared" si="0"/>
         <v>690</v>
@@ -1226,8 +1822,10 @@
       <c r="R14" s="10">
         <v>-1.4630000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="Y14" s="18"/>
+      <c r="Z14" s="18"/>
+    </row>
+    <row r="15" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C15">
         <f t="shared" si="0"/>
         <v>938</v>
@@ -1280,8 +1878,10 @@
       <c r="R15" s="10">
         <v>-1.464</v>
       </c>
-    </row>
-    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="18"/>
+    </row>
+    <row r="16" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C16">
         <f t="shared" si="0"/>
         <v>1208</v>
@@ -1334,8 +1934,10 @@
       <c r="R16" s="10">
         <v>-1.4650000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="Y16" s="18"/>
+      <c r="Z16" s="18"/>
+    </row>
+    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C17">
         <f t="shared" si="0"/>
         <v>1530</v>
@@ -1388,8 +1990,10 @@
       <c r="R17" s="10">
         <v>-1.466</v>
       </c>
-    </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="Y17" s="18"/>
+      <c r="Z17" s="18"/>
+    </row>
+    <row r="18" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C18">
         <f t="shared" si="0"/>
         <v>1860.0000000000002</v>
@@ -1442,8 +2046,10 @@
       <c r="R18" s="10">
         <v>-1.466</v>
       </c>
-    </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="Y18" s="18"/>
+      <c r="Z18" s="18"/>
+    </row>
+    <row r="19" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C19">
         <f t="shared" si="0"/>
         <v>2255</v>
@@ -1496,8 +2102,10 @@
       <c r="R19" s="10">
         <v>-1.468</v>
       </c>
-    </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="Y19" s="18"/>
+      <c r="Z19" s="18"/>
+    </row>
+    <row r="20" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C20">
         <f t="shared" si="0"/>
         <v>2676</v>
@@ -1550,8 +2158,10 @@
       <c r="R20" s="10">
         <v>-1.4690000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="Y20" s="18"/>
+      <c r="Z20" s="18"/>
+    </row>
+    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C21">
         <f t="shared" si="0"/>
         <v>3120</v>
@@ -1604,8 +2214,10 @@
       <c r="R21" s="10">
         <v>-1.47</v>
       </c>
-    </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="Y21" s="18"/>
+      <c r="Z21" s="18"/>
+    </row>
+    <row r="22" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C22">
         <f t="shared" si="0"/>
         <v>3612</v>
@@ -1658,8 +2270,10 @@
       <c r="R22" s="10">
         <v>-1.4710000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="Y22" s="18"/>
+      <c r="Z22" s="18"/>
+    </row>
+    <row r="23" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C23">
         <f t="shared" si="0"/>
         <v>4140</v>
@@ -1712,8 +2326,10 @@
       <c r="R23" s="10">
         <v>-1.4730000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="Y23" s="18"/>
+      <c r="Z23" s="18"/>
+    </row>
+    <row r="24" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C24">
         <f t="shared" si="0"/>
         <v>4688</v>
@@ -1766,8 +2382,10 @@
       <c r="R24" s="10">
         <v>-1.474</v>
       </c>
-    </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="Y24" s="18"/>
+      <c r="Z24" s="18"/>
+    </row>
+    <row r="25" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C25">
         <f t="shared" si="0"/>
         <v>5270</v>
@@ -1820,8 +2438,10 @@
       <c r="R25" s="10">
         <v>-1.476</v>
       </c>
-    </row>
-    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="Y25" s="18"/>
+      <c r="Z25" s="18"/>
+    </row>
+    <row r="26" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C26">
         <f t="shared" si="0"/>
         <v>5868</v>
@@ -1874,8 +2494,10 @@
       <c r="R26" s="10">
         <v>-1.4770000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="Y26" s="18"/>
+      <c r="Z26" s="18"/>
+    </row>
+    <row r="27" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C27">
         <f t="shared" si="0"/>
         <v>6536</v>
@@ -1928,8 +2550,10 @@
       <c r="R27" s="10">
         <v>-1.4790000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y27" s="18"/>
+      <c r="Z27" s="18"/>
+    </row>
+    <row r="28" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28">
         <f t="shared" si="0"/>
         <v>7159.9999999999991</v>
@@ -1982,13 +2606,32 @@
       <c r="R28" s="13">
         <v>-1.4810000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="Y28" s="18"/>
+      <c r="Z28" s="18"/>
+    </row>
+    <row r="29" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="Y29" s="18"/>
+      <c r="Z29" s="18"/>
+    </row>
+    <row r="30" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="Y30" s="18"/>
+      <c r="Z30" s="18"/>
+    </row>
+    <row r="31" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y31" s="18"/>
+      <c r="Z31" s="18"/>
+    </row>
+    <row r="32" spans="3:26" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="Y32" s="18"/>
+      <c r="Z32" s="18"/>
+    </row>
+    <row r="33" spans="5:26" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
         <v>19</v>
       </c>
@@ -2007,8 +2650,22 @@
       <c r="L33" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="O33" t="s">
+        <v>29</v>
+      </c>
+      <c r="P33" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q33" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R33">
+        <v>4</v>
+      </c>
+      <c r="Y33" s="18"/>
+      <c r="Z33" s="18"/>
+    </row>
+    <row r="34" spans="5:26" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
         <v>18</v>
       </c>
@@ -2035,24 +2692,498 @@
       <c r="L34">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="G36" t="s">
+      <c r="O34" s="9">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <f>ROUND($G$37*O34+$H$37,1)</f>
+        <v>0.7</v>
+      </c>
+      <c r="Q34" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="R34">
+        <f>$G$28*G37+H37</f>
+        <v>36.322857142857139</v>
+      </c>
+      <c r="Y34" s="18"/>
+      <c r="Z34" s="18"/>
+    </row>
+    <row r="35" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="O35" s="9">
+        <v>10</v>
+      </c>
+      <c r="P35">
+        <f t="shared" ref="P35:P54" si="4">ROUND($G$37*O35+$H$37,1)</f>
+        <v>2.5</v>
+      </c>
+      <c r="Q35">
+        <v>2.1</v>
+      </c>
+      <c r="Y35" s="18"/>
+      <c r="Z35" s="18"/>
+    </row>
+    <row r="36" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="G36" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="37" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="G37">
+      <c r="O36" s="9">
+        <v>20</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="4"/>
+        <v>4.3</v>
+      </c>
+      <c r="Q36" s="4">
+        <v>4</v>
+      </c>
+      <c r="Y36" s="18"/>
+      <c r="Z36" s="18"/>
+    </row>
+    <row r="37" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="G37" s="19">
         <f>(G34*H34-L34*K34)/(G34*G34-L34*I34)</f>
         <v>0.17787218045112774</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="19">
         <f>(H34-G37*G34)/(L34)</f>
         <v>0.74842105263159053</v>
       </c>
+      <c r="O37" s="9">
+        <v>30</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="4"/>
+        <v>6.1</v>
+      </c>
+      <c r="Q37" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="Y37" s="18"/>
+      <c r="Z37" s="18"/>
+    </row>
+    <row r="38" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="O38" s="9">
+        <v>40</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="4"/>
+        <v>7.9</v>
+      </c>
+      <c r="Q38" s="4">
+        <v>7.8</v>
+      </c>
+      <c r="Y38" s="18"/>
+      <c r="Z38" s="18"/>
+    </row>
+    <row r="39" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="G39" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H39" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="O39" s="9">
+        <v>50</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="4"/>
+        <v>9.6</v>
+      </c>
+      <c r="Q39" s="4">
+        <v>9.6</v>
+      </c>
+      <c r="Y39" s="18"/>
+      <c r="Z39" s="18"/>
+    </row>
+    <row r="40" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="G40" s="19">
+        <f>ROUND(SQRT((L34*(J34-G37*K34-H37*H34))/(18*(L34*I34-G34*G34))),4)</f>
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="H40" s="19">
+        <f>ROUND(G40*SQRT(I34/L34),4)</f>
+        <v>8.3900000000000002E-2</v>
+      </c>
+      <c r="O40" s="9">
+        <v>60</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="4"/>
+        <v>11.4</v>
+      </c>
+      <c r="Q40" s="4">
+        <v>11.5</v>
+      </c>
+      <c r="Y40" s="18"/>
+      <c r="Z40" s="18"/>
+    </row>
+    <row r="41" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="O41" s="9">
+        <v>70</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="4"/>
+        <v>13.2</v>
+      </c>
+      <c r="Q41" s="4">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="42" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="O42" s="9">
+        <v>80</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="Q42" s="4">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="43" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="O43" s="9">
+        <v>90</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="4"/>
+        <v>16.8</v>
+      </c>
+      <c r="Q43" s="4">
+        <v>17</v>
+      </c>
+      <c r="Y43" s="18"/>
+      <c r="Z43" s="18"/>
+    </row>
+    <row r="44" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="F44" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="H44" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I44" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J44" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="O44" s="9">
+        <v>100</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="4"/>
+        <v>18.5</v>
+      </c>
+      <c r="Q44" s="4">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="Y44" s="18"/>
+      <c r="Z44" s="18"/>
+    </row>
+    <row r="45" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="F45" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H45" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I45" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="J45" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="O45" s="9">
+        <v>110</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="4"/>
+        <v>20.3</v>
+      </c>
+      <c r="Q45" s="4">
+        <v>20.5</v>
+      </c>
+      <c r="Y45" s="18"/>
+      <c r="Z45" s="18"/>
+    </row>
+    <row r="46" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="F46" s="19">
+        <v>200</v>
+      </c>
+      <c r="H46" s="19">
+        <f>SQRT(F46*F46*G40*G40+H40+H40)</f>
+        <v>0.43289721643826728</v>
+      </c>
+      <c r="I46" s="19">
+        <f>H46/F47</f>
+        <v>1.1925543152569348E-2</v>
+      </c>
+      <c r="J46" s="19">
+        <f>2*H46</f>
+        <v>0.86579443287653457</v>
+      </c>
+      <c r="O46" s="9">
+        <v>120</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="4"/>
+        <v>22.1</v>
+      </c>
+      <c r="Q46" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="Y46" s="18"/>
+      <c r="Z46" s="18"/>
+    </row>
+    <row r="47" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47" s="19">
+        <f>ROUND(F46*G37+H37,1)</f>
+        <v>36.299999999999997</v>
+      </c>
+      <c r="O47" s="9">
+        <v>130</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="4"/>
+        <v>23.9</v>
+      </c>
+      <c r="Q47" s="4">
+        <v>24</v>
+      </c>
+      <c r="Y47" s="18"/>
+      <c r="Z47" s="18"/>
+    </row>
+    <row r="48" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="O48" s="9">
+        <v>140</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="4"/>
+        <v>25.7</v>
+      </c>
+      <c r="Q48" s="4">
+        <v>25.8</v>
+      </c>
+      <c r="Y48" s="18"/>
+      <c r="Z48" s="18"/>
+    </row>
+    <row r="49" spans="15:26" x14ac:dyDescent="0.25">
+      <c r="O49" s="9">
+        <v>150</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="4"/>
+        <v>27.4</v>
+      </c>
+      <c r="Q49" s="4">
+        <v>27.6</v>
+      </c>
+      <c r="Y49" s="18"/>
+      <c r="Z49" s="18"/>
+    </row>
+    <row r="50" spans="15:26" x14ac:dyDescent="0.25">
+      <c r="O50" s="9">
+        <v>160</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="4"/>
+        <v>29.2</v>
+      </c>
+      <c r="Q50" s="4">
+        <v>29.3</v>
+      </c>
+      <c r="Y50" s="18"/>
+      <c r="Z50" s="18"/>
+    </row>
+    <row r="51" spans="15:26" x14ac:dyDescent="0.25">
+      <c r="O51" s="9">
+        <v>170</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="Q51" s="4">
+        <v>31</v>
+      </c>
+      <c r="Y51" s="18"/>
+      <c r="Z51" s="18"/>
+    </row>
+    <row r="52" spans="15:26" x14ac:dyDescent="0.25">
+      <c r="O52" s="9">
+        <v>180</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="4"/>
+        <v>32.799999999999997</v>
+      </c>
+      <c r="Q52" s="4">
+        <v>32.6</v>
+      </c>
+      <c r="Y52" s="18"/>
+      <c r="Z52" s="18"/>
+    </row>
+    <row r="53" spans="15:26" x14ac:dyDescent="0.25">
+      <c r="O53" s="9">
+        <v>190</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="4"/>
+        <v>34.5</v>
+      </c>
+      <c r="Q53" s="4">
+        <v>34.4</v>
+      </c>
+      <c r="Y53" s="18"/>
+      <c r="Z53" s="18"/>
+    </row>
+    <row r="54" spans="15:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O54" s="11">
+        <v>200</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="4"/>
+        <v>36.299999999999997</v>
+      </c>
+      <c r="Q54" s="12">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="Y54" s="18"/>
+      <c r="Z54" s="18"/>
+    </row>
+    <row r="55" spans="15:26" x14ac:dyDescent="0.25">
+      <c r="Y55" s="18"/>
+      <c r="Z55" s="18"/>
+    </row>
+    <row r="56" spans="15:26" x14ac:dyDescent="0.25">
+      <c r="Y56" s="18"/>
+      <c r="Z56" s="18"/>
+    </row>
+    <row r="57" spans="15:26" x14ac:dyDescent="0.25">
+      <c r="Y57" s="18"/>
+      <c r="Z57" s="18"/>
+    </row>
+    <row r="58" spans="15:26" x14ac:dyDescent="0.25">
+      <c r="Y58" s="18"/>
+      <c r="Z58" s="18"/>
+    </row>
+    <row r="59" spans="15:26" x14ac:dyDescent="0.25">
+      <c r="Y59" s="18"/>
+      <c r="Z59" s="18"/>
+    </row>
+    <row r="60" spans="15:26" x14ac:dyDescent="0.25">
+      <c r="Y60" s="18"/>
+      <c r="Z60" s="18"/>
+    </row>
+    <row r="61" spans="15:26" x14ac:dyDescent="0.25">
+      <c r="Y61" s="18"/>
+      <c r="Z61" s="18"/>
+    </row>
+    <row r="62" spans="15:26" x14ac:dyDescent="0.25">
+      <c r="Y62" s="18"/>
+      <c r="Z62" s="18"/>
+    </row>
+    <row r="63" spans="15:26" x14ac:dyDescent="0.25">
+      <c r="Y63" s="18"/>
+      <c r="Z63" s="18"/>
+    </row>
+    <row r="64" spans="15:26" x14ac:dyDescent="0.25">
+      <c r="Y64" s="18"/>
+      <c r="Z64" s="18"/>
+    </row>
+    <row r="65" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y65" s="18"/>
+      <c r="Z65" s="18"/>
+    </row>
+    <row r="66" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y66" s="18"/>
+      <c r="Z66" s="18"/>
+    </row>
+    <row r="67" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y67" s="18"/>
+      <c r="Z67" s="18"/>
+    </row>
+    <row r="68" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y68" s="18"/>
+      <c r="Z68" s="18"/>
+    </row>
+    <row r="69" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y69" s="18"/>
+      <c r="Z69" s="18"/>
+    </row>
+    <row r="70" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y70" s="18"/>
+      <c r="Z70" s="18"/>
+    </row>
+    <row r="71" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y71" s="18"/>
+      <c r="Z71" s="18"/>
+    </row>
+    <row r="72" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y72" s="18"/>
+      <c r="Z72" s="18"/>
+    </row>
+    <row r="73" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y73" s="18"/>
+      <c r="Z73" s="18"/>
+    </row>
+    <row r="74" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y74" s="18"/>
+      <c r="Z74" s="18"/>
+    </row>
+    <row r="75" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y75" s="18"/>
+      <c r="Z75" s="18"/>
+    </row>
+    <row r="76" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y76" s="18"/>
+      <c r="Z76" s="18"/>
+    </row>
+    <row r="77" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y77" s="18"/>
+      <c r="Z77" s="18"/>
+    </row>
+    <row r="78" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y78" s="18"/>
+      <c r="Z78" s="18"/>
+    </row>
+    <row r="79" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y79" s="18"/>
+      <c r="Z79" s="18"/>
+    </row>
+    <row r="80" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y80" s="18"/>
+      <c r="Z80" s="18"/>
+    </row>
+    <row r="81" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y81" s="18"/>
+      <c r="Z81" s="18"/>
+    </row>
+    <row r="82" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y82" s="18"/>
+      <c r="Z82" s="18"/>
+    </row>
+    <row r="83" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y83" s="18"/>
+      <c r="Z83" s="18"/>
+    </row>
+    <row r="84" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y84" s="18"/>
+      <c r="Z84" s="18"/>
+    </row>
+    <row r="85" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y85" s="18"/>
+      <c r="Z85" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Skonczono obliczenia z Halla
</commit_message>
<xml_diff>
--- a/FIZ2/Halla.xlsx
+++ b/FIZ2/Halla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kamil\Desktop\Stary Folder\studia_git\FIZ2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FD1598-101F-4530-A56E-17247E67515B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93350134-B612-4289-8627-4571814B01AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22106E2D-535D-4D61-8847-61EECC787C3F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="85">
   <si>
     <t>B[mT]</t>
   </si>
@@ -165,14 +165,142 @@
   </si>
   <si>
     <t>U(Uh)</t>
+  </si>
+  <si>
+    <t>AD8</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>mT</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>mV</t>
+  </si>
+  <si>
+    <t>mC</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>m^-3</t>
+  </si>
+  <si>
+    <t>AD9</t>
+  </si>
+  <si>
+    <t>u(I)</t>
+  </si>
+  <si>
+    <t>u(B)</t>
+  </si>
+  <si>
+    <t>uc,r(n)</t>
+  </si>
+  <si>
+    <t>uc(n)</t>
+  </si>
+  <si>
+    <t>U(n)</t>
+  </si>
+  <si>
+    <t>AD10</t>
+  </si>
+  <si>
+    <t>AD11</t>
+  </si>
+  <si>
+    <t>AD12</t>
+  </si>
+  <si>
+    <t>Upsr</t>
+  </si>
+  <si>
+    <t>AD13</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>miu</t>
+  </si>
+  <si>
+    <t>m^2/Vs</t>
+  </si>
+  <si>
+    <t>AD14</t>
+  </si>
+  <si>
+    <t>uc,r(miu)</t>
+  </si>
+  <si>
+    <t>deltaUP</t>
+  </si>
+  <si>
+    <t>u(Up)</t>
+  </si>
+  <si>
+    <t>AD15</t>
+  </si>
+  <si>
+    <t>uc(miu)</t>
+  </si>
+  <si>
+    <t>AD16</t>
+  </si>
+  <si>
+    <t>U(miu)</t>
+  </si>
+  <si>
+    <t>u(Uh)</t>
+  </si>
+  <si>
+    <t>deltaU</t>
+  </si>
+  <si>
+    <t>u(U)</t>
+  </si>
+  <si>
+    <t>delta Uh/Up</t>
+  </si>
+  <si>
+    <t>dla B=200</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -184,7 +312,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +322,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -394,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -410,11 +544,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -430,6 +567,1027 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$T$60</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Uh[V]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$S$61:$S$81</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$T$61:$T$81</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>27.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>32.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>34.4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>35.799999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A0C8-40F8-9DBF-B78AB7967D2F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1095300447"/>
+        <c:axId val="2037901343"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1095300447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2037901343"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2037901343"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1095300447"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>621926</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>158002</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>218514</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>43702</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54E21627-E69A-3EFA-63A8-071396198BD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -729,32 +1887,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A447AA0A-D447-4B02-AC14-94CF8529AAB0}">
-  <dimension ref="C1:DD85"/>
+  <dimension ref="C4:DD81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44:J46"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U45" sqref="U45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.5703125" customWidth="1"/>
-    <col min="24" max="108" width="5" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" customWidth="1"/>
+    <col min="24" max="24" width="8.85546875" customWidth="1"/>
+    <col min="25" max="26" width="5" customWidth="1"/>
+    <col min="27" max="29" width="10.7109375" customWidth="1"/>
+    <col min="30" max="108" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:108" x14ac:dyDescent="0.25">
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-    </row>
-    <row r="2" spans="3:108" x14ac:dyDescent="0.25">
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="18"/>
-    </row>
-    <row r="3" spans="3:108" x14ac:dyDescent="0.25">
-      <c r="Y3" s="18"/>
-      <c r="Z3" s="18"/>
-    </row>
     <row r="4" spans="3:108" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T4" t="s">
         <v>9</v>
@@ -1363,8 +2515,6 @@
       <c r="V6" t="s">
         <v>10</v>
       </c>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="18"/>
     </row>
     <row r="7" spans="3:108" x14ac:dyDescent="0.25">
       <c r="G7" s="9" t="s">
@@ -1412,8 +2562,6 @@
       <c r="V7" t="s">
         <v>8</v>
       </c>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="18"/>
     </row>
     <row r="8" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C8">
@@ -1428,9 +2576,9 @@
         <f>H8*H8</f>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="15">
         <f>G8*$G$37+$H$37</f>
-        <v>0.74842105263159053</v>
+        <v>0.74550000000000005</v>
       </c>
       <c r="G8" s="9">
         <v>0</v>
@@ -1477,8 +2625,6 @@
       <c r="V8" t="s">
         <v>3</v>
       </c>
-      <c r="Y8" s="18"/>
-      <c r="Z8" s="18"/>
     </row>
     <row r="9" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C9">
@@ -1493,9 +2639,9 @@
         <f t="shared" ref="E9:E28" si="2">H9*H9</f>
         <v>4.41</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="15">
         <f t="shared" ref="F9:F28" si="3">G9*$G$37+$H$37</f>
-        <v>2.5271428571428678</v>
+        <v>2.5244999999999997</v>
       </c>
       <c r="G9" s="9">
         <v>10</v>
@@ -1542,8 +2688,9 @@
       <c r="V9" t="s">
         <v>16</v>
       </c>
-      <c r="Y9" s="18"/>
-      <c r="Z9" s="18"/>
+      <c r="W9">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="10" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C10">
@@ -1558,9 +2705,9 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="15">
         <f t="shared" si="3"/>
-        <v>4.3058646616541454</v>
+        <v>4.3034999999999997</v>
       </c>
       <c r="G10" s="9">
         <v>20</v>
@@ -1598,8 +2745,13 @@
       <c r="R10" s="10">
         <v>-1.462</v>
       </c>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="18"/>
+      <c r="W10">
+        <f>G28*W9</f>
+        <v>4</v>
+      </c>
+      <c r="X10" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C11">
@@ -1614,9 +2766,9 @@
         <f t="shared" si="2"/>
         <v>34.81</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="15">
         <f t="shared" si="3"/>
-        <v>6.0845864661654225</v>
+        <v>6.0824999999999996</v>
       </c>
       <c r="G11" s="9">
         <v>30</v>
@@ -1654,8 +2806,13 @@
       <c r="R11" s="10">
         <v>-1.462</v>
       </c>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="18"/>
+      <c r="T11" t="s">
+        <v>74</v>
+      </c>
+      <c r="U11">
+        <v>1E-3</v>
+      </c>
+      <c r="X11" s="19"/>
     </row>
     <row r="12" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C12">
@@ -1670,9 +2827,9 @@
         <f t="shared" si="2"/>
         <v>60.839999999999996</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="15">
         <f t="shared" si="3"/>
-        <v>7.8633082706766997</v>
+        <v>7.8614999999999995</v>
       </c>
       <c r="G12" s="9">
         <v>40</v>
@@ -1710,8 +2867,9 @@
       <c r="R12" s="10">
         <v>-1.462</v>
       </c>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="18"/>
+      <c r="V12" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="13" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C13">
@@ -1726,9 +2884,9 @@
         <f t="shared" si="2"/>
         <v>92.16</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="15">
         <f t="shared" si="3"/>
-        <v>9.6420300751879768</v>
+        <v>9.6404999999999994</v>
       </c>
       <c r="G13" s="9">
         <v>50</v>
@@ -1766,8 +2924,23 @@
       <c r="R13" s="10">
         <v>-1.4630000000000001</v>
       </c>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
+      <c r="T13" t="s">
+        <v>83</v>
+      </c>
+      <c r="U13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="V13">
+        <f>H28*U13</f>
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="W13" t="s">
+        <v>80</v>
+      </c>
+      <c r="X13">
+        <f>ROUND(V13/SQRT(3),1)</f>
+        <v>0.1</v>
+      </c>
     </row>
     <row r="14" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C14">
@@ -1782,9 +2955,9 @@
         <f t="shared" si="2"/>
         <v>132.25</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="15">
         <f t="shared" si="3"/>
-        <v>11.420751879699255</v>
+        <v>11.419499999999999</v>
       </c>
       <c r="G14" s="9">
         <v>60</v>
@@ -1822,8 +2995,17 @@
       <c r="R14" s="10">
         <v>-1.4630000000000001</v>
       </c>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="18"/>
+      <c r="V14">
+        <f>I28*U13</f>
+        <v>6.6500000000000005E-3</v>
+      </c>
+      <c r="W14" t="s">
+        <v>75</v>
+      </c>
+      <c r="X14">
+        <f>ROUND(V14/SQRT(3),3)</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="15" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C15">
@@ -1838,9 +3020,9 @@
         <f t="shared" si="2"/>
         <v>179.56</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="15">
         <f t="shared" si="3"/>
-        <v>13.199473684210531</v>
+        <v>13.198499999999999</v>
       </c>
       <c r="G15" s="9">
         <v>70</v>
@@ -1878,8 +3060,6 @@
       <c r="R15" s="10">
         <v>-1.464</v>
       </c>
-      <c r="Y15" s="18"/>
-      <c r="Z15" s="18"/>
     </row>
     <row r="16" spans="3:108" x14ac:dyDescent="0.25">
       <c r="C16">
@@ -1894,9 +3074,9 @@
         <f t="shared" si="2"/>
         <v>228.01</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="15">
         <f t="shared" si="3"/>
-        <v>14.978195488721809</v>
+        <v>14.977499999999999</v>
       </c>
       <c r="G16" s="9">
         <v>80</v>
@@ -1934,10 +3114,8 @@
       <c r="R16" s="10">
         <v>-1.4650000000000001</v>
       </c>
-      <c r="Y16" s="18"/>
-      <c r="Z16" s="18"/>
-    </row>
-    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C17">
         <f t="shared" si="0"/>
         <v>1530</v>
@@ -1950,9 +3128,9 @@
         <f t="shared" si="2"/>
         <v>289</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="15">
         <f t="shared" si="3"/>
-        <v>16.756917293233087</v>
+        <v>16.756499999999999</v>
       </c>
       <c r="G17" s="9">
         <v>90</v>
@@ -1990,10 +3168,8 @@
       <c r="R17" s="10">
         <v>-1.466</v>
       </c>
-      <c r="Y17" s="18"/>
-      <c r="Z17" s="18"/>
-    </row>
-    <row r="18" spans="3:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C18">
         <f t="shared" si="0"/>
         <v>1860.0000000000002</v>
@@ -2006,9 +3182,9 @@
         <f t="shared" si="2"/>
         <v>345.96000000000004</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="15">
         <f t="shared" si="3"/>
-        <v>18.535639097744365</v>
+        <v>18.535499999999999</v>
       </c>
       <c r="G18" s="9">
         <v>100</v>
@@ -2046,10 +3222,18 @@
       <c r="R18" s="10">
         <v>-1.466</v>
       </c>
-      <c r="Y18" s="18"/>
-      <c r="Z18" s="18"/>
-    </row>
-    <row r="19" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="U18" t="s">
+        <v>58</v>
+      </c>
+      <c r="V18">
+        <f>ROUND(U7/SQRT(3),4)</f>
+        <v>0.57740000000000002</v>
+      </c>
+      <c r="W18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C19">
         <f t="shared" si="0"/>
         <v>2255</v>
@@ -2062,9 +3246,9 @@
         <f t="shared" si="2"/>
         <v>420.25</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="15">
         <f t="shared" si="3"/>
-        <v>20.314360902255643</v>
+        <v>20.314499999999999</v>
       </c>
       <c r="G19" s="9">
         <v>110</v>
@@ -2102,10 +3286,18 @@
       <c r="R19" s="10">
         <v>-1.468</v>
       </c>
-      <c r="Y19" s="18"/>
-      <c r="Z19" s="18"/>
-    </row>
-    <row r="20" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="U19" t="s">
+        <v>59</v>
+      </c>
+      <c r="V19">
+        <f>ROUND(W10/SQRT(3),4)</f>
+        <v>2.3094000000000001</v>
+      </c>
+      <c r="W19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C20">
         <f t="shared" si="0"/>
         <v>2676</v>
@@ -2118,9 +3310,9 @@
         <f t="shared" si="2"/>
         <v>497.29</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="15">
         <f t="shared" si="3"/>
-        <v>22.093082706766921</v>
+        <v>22.093499999999999</v>
       </c>
       <c r="G20" s="9">
         <v>120</v>
@@ -2158,10 +3350,18 @@
       <c r="R20" s="10">
         <v>-1.4690000000000001</v>
       </c>
-      <c r="Y20" s="18"/>
-      <c r="Z20" s="18"/>
-    </row>
-    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="U20" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="V20" s="17">
+        <f>H46</f>
+        <v>0.36030000000000001</v>
+      </c>
+      <c r="W20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C21">
         <f t="shared" si="0"/>
         <v>3120</v>
@@ -2174,9 +3374,9 @@
         <f t="shared" si="2"/>
         <v>576</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="15">
         <f t="shared" si="3"/>
-        <v>23.871804511278199</v>
+        <v>23.872499999999999</v>
       </c>
       <c r="G21" s="9">
         <v>130</v>
@@ -2214,10 +3414,8 @@
       <c r="R21" s="10">
         <v>-1.47</v>
       </c>
-      <c r="Y21" s="18"/>
-      <c r="Z21" s="18"/>
-    </row>
-    <row r="22" spans="3:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C22">
         <f t="shared" si="0"/>
         <v>3612</v>
@@ -2230,9 +3428,9 @@
         <f t="shared" si="2"/>
         <v>665.64</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="15">
         <f t="shared" si="3"/>
-        <v>25.650526315789474</v>
+        <v>25.651499999999999</v>
       </c>
       <c r="G22" s="9">
         <v>140</v>
@@ -2249,7 +3447,7 @@
       <c r="K22" s="4">
         <v>-25.4</v>
       </c>
-      <c r="L22" s="15">
+      <c r="L22" s="20">
         <v>1.333</v>
       </c>
       <c r="M22" s="8">
@@ -2270,10 +3468,8 @@
       <c r="R22" s="10">
         <v>-1.4710000000000001</v>
       </c>
-      <c r="Y22" s="18"/>
-      <c r="Z22" s="18"/>
-    </row>
-    <row r="23" spans="3:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C23">
         <f t="shared" si="0"/>
         <v>4140</v>
@@ -2286,9 +3482,9 @@
         <f t="shared" si="2"/>
         <v>761.7600000000001</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="15">
         <f t="shared" si="3"/>
-        <v>27.429248120300752</v>
+        <v>27.430499999999999</v>
       </c>
       <c r="G23" s="9">
         <v>150</v>
@@ -2305,7 +3501,7 @@
       <c r="K23" s="4">
         <v>-27.2</v>
       </c>
-      <c r="L23" s="15">
+      <c r="L23" s="20">
         <v>1.3340000000000001</v>
       </c>
       <c r="M23" s="8">
@@ -2326,10 +3522,17 @@
       <c r="R23" s="10">
         <v>-1.4730000000000001</v>
       </c>
-      <c r="Y23" s="18"/>
-      <c r="Z23" s="18"/>
-    </row>
-    <row r="24" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="U23" t="s">
+        <v>57</v>
+      </c>
+      <c r="V23" t="s">
+        <v>63</v>
+      </c>
+      <c r="W23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C24">
         <f t="shared" si="0"/>
         <v>4688</v>
@@ -2342,9 +3545,9 @@
         <f t="shared" si="2"/>
         <v>858.49</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="15">
         <f t="shared" si="3"/>
-        <v>29.20796992481203</v>
+        <v>29.209499999999998</v>
       </c>
       <c r="G24" s="9">
         <v>160</v>
@@ -2361,7 +3564,7 @@
       <c r="K24" s="4">
         <v>-28.9</v>
       </c>
-      <c r="L24" s="15">
+      <c r="L24" s="20">
         <v>1.3360000000000001</v>
       </c>
       <c r="M24" s="8">
@@ -2382,10 +3585,17 @@
       <c r="R24" s="10">
         <v>-1.474</v>
       </c>
-      <c r="Y24" s="18"/>
-      <c r="Z24" s="18"/>
-    </row>
-    <row r="25" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="U24" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="V24" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="W24" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C25">
         <f t="shared" si="0"/>
         <v>5270</v>
@@ -2398,9 +3608,9 @@
         <f t="shared" si="2"/>
         <v>961</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="15">
         <f t="shared" si="3"/>
-        <v>30.986691729323308</v>
+        <v>30.988500000000002</v>
       </c>
       <c r="G25" s="9">
         <v>170</v>
@@ -2417,7 +3627,7 @@
       <c r="K25" s="4">
         <v>-30.8</v>
       </c>
-      <c r="L25" s="15">
+      <c r="L25" s="20">
         <v>1.337</v>
       </c>
       <c r="M25" s="8">
@@ -2438,10 +3648,20 @@
       <c r="R25" s="10">
         <v>-1.476</v>
       </c>
-      <c r="Y25" s="18"/>
-      <c r="Z25" s="18"/>
-    </row>
-    <row r="26" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="U25" s="16">
+        <f>ROUND(SQRT((X13/H28)*(X13/H28)+(V19/G28)*(V19/G28)+(V18/H5)*(V18/H5)),4)</f>
+        <v>2.2599999999999999E-2</v>
+      </c>
+      <c r="V25" s="16">
+        <f>ROUND(U25*K59,4)</f>
+        <v>2.36436298202665E+16</v>
+      </c>
+      <c r="W25" s="16">
+        <f>2*U25</f>
+        <v>4.5199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C26">
         <f t="shared" si="0"/>
         <v>5868</v>
@@ -2454,9 +3674,9 @@
         <f t="shared" si="2"/>
         <v>1062.76</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="15">
         <f t="shared" si="3"/>
-        <v>32.765413533834582</v>
+        <v>32.767499999999998</v>
       </c>
       <c r="G26" s="9">
         <v>180</v>
@@ -2473,7 +3693,7 @@
       <c r="K26" s="4">
         <v>-32.4</v>
       </c>
-      <c r="L26" s="15">
+      <c r="L26" s="20">
         <v>1.339</v>
       </c>
       <c r="M26" s="8">
@@ -2494,10 +3714,8 @@
       <c r="R26" s="10">
         <v>-1.4770000000000001</v>
       </c>
-      <c r="Y26" s="18"/>
-      <c r="Z26" s="18"/>
-    </row>
-    <row r="27" spans="3:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C27">
         <f t="shared" si="0"/>
         <v>6536</v>
@@ -2510,9 +3728,9 @@
         <f t="shared" si="2"/>
         <v>1183.3599999999999</v>
       </c>
-      <c r="F27" s="17">
+      <c r="F27" s="15">
         <f t="shared" si="3"/>
-        <v>34.54413533834586</v>
+        <v>34.546500000000002</v>
       </c>
       <c r="G27" s="9">
         <v>190</v>
@@ -2529,7 +3747,7 @@
       <c r="K27" s="4">
         <v>-34</v>
       </c>
-      <c r="L27" s="15">
+      <c r="L27" s="20">
         <v>1.34</v>
       </c>
       <c r="M27" s="8">
@@ -2550,10 +3768,8 @@
       <c r="R27" s="10">
         <v>-1.4790000000000001</v>
       </c>
-      <c r="Y27" s="18"/>
-      <c r="Z27" s="18"/>
-    </row>
-    <row r="28" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28">
         <f t="shared" si="0"/>
         <v>7159.9999999999991</v>
@@ -2566,9 +3782,9 @@
         <f t="shared" si="2"/>
         <v>1281.6399999999999</v>
       </c>
-      <c r="F28" s="17">
+      <c r="F28" s="15">
         <f t="shared" si="3"/>
-        <v>36.322857142857139</v>
+        <v>36.325499999999998</v>
       </c>
       <c r="G28" s="11">
         <v>200</v>
@@ -2585,7 +3801,7 @@
       <c r="K28" s="12">
         <v>-36</v>
       </c>
-      <c r="L28" s="16">
+      <c r="L28" s="21">
         <v>1.3420000000000001</v>
       </c>
       <c r="M28" s="14">
@@ -2606,32 +3822,110 @@
       <c r="R28" s="13">
         <v>-1.4810000000000001</v>
       </c>
-      <c r="Y28" s="18"/>
-      <c r="Z28" s="18"/>
-    </row>
-    <row r="29" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="Y29" s="18"/>
-      <c r="Z29" s="18"/>
-    </row>
-    <row r="30" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="Y30" s="18"/>
-      <c r="Z30" s="18"/>
-    </row>
-    <row r="31" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="U28" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="V28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="U29" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="V29" t="s">
+        <v>44</v>
+      </c>
+      <c r="W29">
+        <v>30</v>
+      </c>
+      <c r="X29" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB29">
+        <f>30/1000</f>
+        <v>0.03</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="U30" s="18">
+        <f>SUM(I8:I28)/21</f>
+        <v>1.3199999999999998</v>
+      </c>
+      <c r="V30" t="s">
+        <v>68</v>
+      </c>
+      <c r="W30">
+        <v>1.32</v>
+      </c>
+      <c r="X30" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB30">
+        <v>1.32</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="3:29" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
         <v>31</v>
       </c>
-      <c r="Y31" s="18"/>
-      <c r="Z31" s="18"/>
-    </row>
-    <row r="32" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="V31" t="s">
+        <v>69</v>
+      </c>
+      <c r="W31">
+        <v>20</v>
+      </c>
+      <c r="X31" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB31">
+        <f>20/1000</f>
+        <v>0.02</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="3:29" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
         <v>17</v>
       </c>
-      <c r="Y32" s="18"/>
-      <c r="Z32" s="18"/>
-    </row>
-    <row r="33" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="V32" t="s">
+        <v>26</v>
+      </c>
+      <c r="W32">
+        <v>10</v>
+      </c>
+      <c r="X32" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB32">
+        <f>10/1000</f>
+        <v>0.01</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="5:29" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
         <v>19</v>
       </c>
@@ -2662,10 +3956,27 @@
       <c r="R33">
         <v>4</v>
       </c>
-      <c r="Y33" s="18"/>
-      <c r="Z33" s="18"/>
-    </row>
-    <row r="34" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="V33" t="s">
+        <v>49</v>
+      </c>
+      <c r="W33">
+        <v>1</v>
+      </c>
+      <c r="X33" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB33">
+        <f>1/1000</f>
+        <v>1E-3</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="5:29" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
         <v>18</v>
       </c>
@@ -2704,12 +4015,30 @@
       </c>
       <c r="R34">
         <f>$G$28*G37+H37</f>
-        <v>36.322857142857139</v>
-      </c>
-      <c r="Y34" s="18"/>
-      <c r="Z34" s="18"/>
-    </row>
-    <row r="35" spans="5:26" x14ac:dyDescent="0.25">
+        <v>36.325499999999998</v>
+      </c>
+      <c r="V34" t="s">
+        <v>48</v>
+      </c>
+      <c r="W34">
+        <f>1.602*(10^(-19))</f>
+        <v>1.602E-19</v>
+      </c>
+      <c r="X34" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB34">
+        <f>1.602*(10^(-19))</f>
+        <v>1.602E-19</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="5:29" x14ac:dyDescent="0.25">
       <c r="O35" s="9">
         <v>10</v>
       </c>
@@ -2720,14 +4049,30 @@
       <c r="Q35">
         <v>2.1</v>
       </c>
-      <c r="Y35" s="18"/>
-      <c r="Z35" s="18"/>
-    </row>
-    <row r="36" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="G36" s="19" t="s">
+      <c r="V35" t="s">
+        <v>24</v>
+      </c>
+      <c r="W35">
+        <v>1.046178310631264E+18</v>
+      </c>
+      <c r="X35" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB35">
+        <v>1.046178310631264E+18</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="G36" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H36" s="19" t="s">
+      <c r="H36" s="16" t="s">
         <v>26</v>
       </c>
       <c r="O36" s="9">
@@ -2740,17 +4085,39 @@
       <c r="Q36" s="4">
         <v>4</v>
       </c>
-      <c r="Y36" s="18"/>
-      <c r="Z36" s="18"/>
-    </row>
-    <row r="37" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="G37" s="19">
-        <f>(G34*H34-L34*K34)/(G34*G34-L34*I34)</f>
-        <v>0.17787218045112774</v>
-      </c>
-      <c r="H37" s="19">
-        <f>(H34-G37*G34)/(L34)</f>
-        <v>0.74842105263159053</v>
+      <c r="V36" t="s">
+        <v>40</v>
+      </c>
+      <c r="W36">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="X36" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB36">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="G37" s="16">
+        <f>ROUND((G34*H34-L34*K34)/(G34*G34-L34*I34),4)</f>
+        <v>0.1779</v>
+      </c>
+      <c r="H37" s="16">
+        <f>ROUND((H34-G37*G34)/(L34),4)</f>
+        <v>0.74550000000000005</v>
+      </c>
+      <c r="J37" t="s">
+        <v>33</v>
+      </c>
+      <c r="K37" t="s">
+        <v>40</v>
       </c>
       <c r="O37" s="9">
         <v>30</v>
@@ -2762,12 +4129,36 @@
       <c r="Q37" s="4">
         <v>5.9</v>
       </c>
-      <c r="Y37" s="18"/>
-      <c r="Z37" s="18"/>
-    </row>
-    <row r="38" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
+      <c r="V37" t="s">
+        <v>33</v>
+      </c>
+      <c r="W37">
+        <v>200</v>
+      </c>
+      <c r="X37" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB37">
+        <f>200/1000</f>
+        <v>0.2</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="J38">
+        <v>10</v>
+      </c>
+      <c r="K38">
+        <f>ROUND($G$37*J38+$H$37,1)</f>
+        <v>2.5</v>
+      </c>
       <c r="O38" s="9">
         <v>40</v>
       </c>
@@ -2778,15 +4169,20 @@
       <c r="Q38" s="4">
         <v>7.8</v>
       </c>
-      <c r="Y38" s="18"/>
-      <c r="Z38" s="18"/>
-    </row>
-    <row r="39" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="G39" s="19" t="s">
+    </row>
+    <row r="39" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="G39" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="H39" s="19" t="s">
+      <c r="H39" s="16" t="s">
         <v>37</v>
+      </c>
+      <c r="J39">
+        <v>200</v>
+      </c>
+      <c r="K39">
+        <f>ROUND($G$37*J39+$H$37,1)</f>
+        <v>36.299999999999997</v>
       </c>
       <c r="O39" s="9">
         <v>50</v>
@@ -2798,17 +4194,25 @@
       <c r="Q39" s="4">
         <v>9.6</v>
       </c>
-      <c r="Y39" s="18"/>
-      <c r="Z39" s="18"/>
-    </row>
-    <row r="40" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="G40" s="19">
+      <c r="AA39" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB39" s="16">
+        <f>ROUND((AB36*AB31)/(AB30*AB32*AB37),4)</f>
+        <v>271.21210000000002</v>
+      </c>
+      <c r="AC39" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="G40" s="16">
         <f>ROUND(SQRT((L34*(J34-G37*K34-H37*H34))/(18*(L34*I34-G34*G34))),4)</f>
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="H40" s="19">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H40" s="16">
         <f>ROUND(G40*SQRT(I34/L34),4)</f>
-        <v>8.3900000000000002E-2</v>
+        <v>5.9900000000000002E-2</v>
       </c>
       <c r="O40" s="9">
         <v>60</v>
@@ -2820,10 +4224,8 @@
       <c r="Q40" s="4">
         <v>11.5</v>
       </c>
-      <c r="Y40" s="18"/>
-      <c r="Z40" s="18"/>
-    </row>
-    <row r="41" spans="5:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="5:29" x14ac:dyDescent="0.25">
       <c r="O41" s="9">
         <v>70</v>
       </c>
@@ -2835,7 +4237,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="42" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:29" x14ac:dyDescent="0.25">
       <c r="O42" s="9">
         <v>80</v>
       </c>
@@ -2846,8 +4248,17 @@
       <c r="Q42" s="4">
         <v>15.1</v>
       </c>
-    </row>
-    <row r="43" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="U42" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="V42" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="W42" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="5:29" x14ac:dyDescent="0.25">
       <c r="O43" s="9">
         <v>90</v>
       </c>
@@ -2858,20 +4269,27 @@
       <c r="Q43" s="4">
         <v>17</v>
       </c>
-      <c r="Y43" s="18"/>
-      <c r="Z43" s="18"/>
-    </row>
-    <row r="44" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="F44" s="19" t="s">
+      <c r="U43" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="V43" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="W43" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="F44" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="H44" s="19" t="s">
+      <c r="H44" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I44" s="19" t="s">
+      <c r="I44" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="J44" s="19" t="s">
+      <c r="J44" s="16" t="s">
         <v>41</v>
       </c>
       <c r="O44" s="9">
@@ -2884,20 +4302,30 @@
       <c r="Q44" s="4">
         <v>18.600000000000001</v>
       </c>
-      <c r="Y44" s="18"/>
-      <c r="Z44" s="18"/>
-    </row>
-    <row r="45" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="F45" s="19" t="s">
+      <c r="U44" s="16">
+        <f>ROUND(SQRT((V20/H28)*(V20/H28)+(X14/I28)*(X14/I28)+(V19/G28)*(V19/G28)),4)</f>
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="V44" s="16">
+        <f>ROUND(U44*AB39,4)</f>
+        <v>4.2309000000000001</v>
+      </c>
+      <c r="W44" s="16">
+        <f>2*U44</f>
+        <v>3.1199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="F45" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="H45" s="19" t="s">
+      <c r="H45" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="I45" s="19" t="s">
+      <c r="I45" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J45" s="19" t="s">
+      <c r="J45" s="16" t="s">
         <v>42</v>
       </c>
       <c r="O45" s="9">
@@ -2910,24 +4338,22 @@
       <c r="Q45" s="4">
         <v>20.5</v>
       </c>
-      <c r="Y45" s="18"/>
-      <c r="Z45" s="18"/>
-    </row>
-    <row r="46" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="F46" s="19">
+    </row>
+    <row r="46" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="F46" s="16">
         <v>200</v>
       </c>
-      <c r="H46" s="19">
-        <f>SQRT(F46*F46*G40*G40+H40+H40)</f>
-        <v>0.43289721643826728</v>
-      </c>
-      <c r="I46" s="19">
-        <f>H46/F47</f>
-        <v>1.1925543152569348E-2</v>
-      </c>
-      <c r="J46" s="19">
-        <f>2*H46</f>
-        <v>0.86579443287653457</v>
+      <c r="H46" s="16">
+        <f>ROUND(SQRT(F46*F46*G40*G40+H40+H40),4)</f>
+        <v>0.36030000000000001</v>
+      </c>
+      <c r="I46" s="16">
+        <f>ROUND(H46/F47,4)</f>
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="J46" s="16">
+        <f>ROUND(2*H46,4)</f>
+        <v>0.72060000000000002</v>
       </c>
       <c r="O46" s="9">
         <v>120</v>
@@ -2939,14 +4365,12 @@
       <c r="Q46" s="4">
         <v>22.3</v>
       </c>
-      <c r="Y46" s="18"/>
-      <c r="Z46" s="18"/>
-    </row>
-    <row r="47" spans="5:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
         <v>40</v>
       </c>
-      <c r="F47" s="19">
+      <c r="F47" s="16">
         <f>ROUND(F46*G37+H37,1)</f>
         <v>36.299999999999997</v>
       </c>
@@ -2960,10 +4384,8 @@
       <c r="Q47" s="4">
         <v>24</v>
       </c>
-      <c r="Y47" s="18"/>
-      <c r="Z47" s="18"/>
-    </row>
-    <row r="48" spans="5:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="5:29" x14ac:dyDescent="0.25">
       <c r="O48" s="9">
         <v>140</v>
       </c>
@@ -2974,10 +4396,8 @@
       <c r="Q48" s="4">
         <v>25.8</v>
       </c>
-      <c r="Y48" s="18"/>
-      <c r="Z48" s="18"/>
-    </row>
-    <row r="49" spans="15:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="6:27" x14ac:dyDescent="0.25">
       <c r="O49" s="9">
         <v>150</v>
       </c>
@@ -2988,10 +4408,8 @@
       <c r="Q49" s="4">
         <v>27.6</v>
       </c>
-      <c r="Y49" s="18"/>
-      <c r="Z49" s="18"/>
-    </row>
-    <row r="50" spans="15:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="6:27" x14ac:dyDescent="0.25">
       <c r="O50" s="9">
         <v>160</v>
       </c>
@@ -3002,10 +4420,11 @@
       <c r="Q50" s="4">
         <v>29.3</v>
       </c>
-      <c r="Y50" s="18"/>
-      <c r="Z50" s="18"/>
-    </row>
-    <row r="51" spans="15:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>43</v>
+      </c>
       <c r="O51" s="9">
         <v>170</v>
       </c>
@@ -3016,10 +4435,27 @@
       <c r="Q51" s="4">
         <v>31</v>
       </c>
-      <c r="Y51" s="18"/>
-      <c r="Z51" s="18"/>
-    </row>
-    <row r="52" spans="15:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>44</v>
+      </c>
+      <c r="G52">
+        <v>30</v>
+      </c>
+      <c r="H52" t="s">
+        <v>8</v>
+      </c>
+      <c r="J52" t="s">
+        <v>44</v>
+      </c>
+      <c r="K52">
+        <f>30/1000</f>
+        <v>0.03</v>
+      </c>
+      <c r="L52" t="s">
+        <v>53</v>
+      </c>
       <c r="O52" s="9">
         <v>180</v>
       </c>
@@ -3030,10 +4466,27 @@
       <c r="Q52" s="4">
         <v>32.6</v>
       </c>
-      <c r="Y52" s="18"/>
-      <c r="Z52" s="18"/>
-    </row>
-    <row r="53" spans="15:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>33</v>
+      </c>
+      <c r="G53">
+        <v>200</v>
+      </c>
+      <c r="H53" t="s">
+        <v>45</v>
+      </c>
+      <c r="J53" t="s">
+        <v>33</v>
+      </c>
+      <c r="K53">
+        <f>200/1000</f>
+        <v>0.2</v>
+      </c>
+      <c r="L53" t="s">
+        <v>54</v>
+      </c>
       <c r="O53" s="9">
         <v>190</v>
       </c>
@@ -3044,10 +4497,27 @@
       <c r="Q53" s="4">
         <v>34.4</v>
       </c>
-      <c r="Y53" s="18"/>
-      <c r="Z53" s="18"/>
-    </row>
-    <row r="54" spans="15:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="6:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F54" t="s">
+        <v>46</v>
+      </c>
+      <c r="G54">
+        <f>35.8*1000</f>
+        <v>35800</v>
+      </c>
+      <c r="H54" t="s">
+        <v>51</v>
+      </c>
+      <c r="J54" t="s">
+        <v>46</v>
+      </c>
+      <c r="K54">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="L54" t="s">
+        <v>47</v>
+      </c>
       <c r="O54" s="11">
         <v>200</v>
       </c>
@@ -3058,134 +4528,452 @@
       <c r="Q54" s="12">
         <v>35.799999999999997</v>
       </c>
-      <c r="Y54" s="18"/>
-      <c r="Z54" s="18"/>
-    </row>
-    <row r="55" spans="15:26" x14ac:dyDescent="0.25">
-      <c r="Y55" s="18"/>
-      <c r="Z55" s="18"/>
-    </row>
-    <row r="56" spans="15:26" x14ac:dyDescent="0.25">
-      <c r="Y56" s="18"/>
-      <c r="Z56" s="18"/>
-    </row>
-    <row r="57" spans="15:26" x14ac:dyDescent="0.25">
-      <c r="Y57" s="18"/>
-      <c r="Z57" s="18"/>
-    </row>
-    <row r="58" spans="15:26" x14ac:dyDescent="0.25">
-      <c r="Y58" s="18"/>
-      <c r="Z58" s="18"/>
-    </row>
-    <row r="59" spans="15:26" x14ac:dyDescent="0.25">
-      <c r="Y59" s="18"/>
-      <c r="Z59" s="18"/>
-    </row>
-    <row r="60" spans="15:26" x14ac:dyDescent="0.25">
-      <c r="Y60" s="18"/>
-      <c r="Z60" s="18"/>
-    </row>
-    <row r="61" spans="15:26" x14ac:dyDescent="0.25">
-      <c r="Y61" s="18"/>
-      <c r="Z61" s="18"/>
-    </row>
-    <row r="62" spans="15:26" x14ac:dyDescent="0.25">
-      <c r="Y62" s="18"/>
-      <c r="Z62" s="18"/>
-    </row>
-    <row r="63" spans="15:26" x14ac:dyDescent="0.25">
-      <c r="Y63" s="18"/>
-      <c r="Z63" s="18"/>
-    </row>
-    <row r="64" spans="15:26" x14ac:dyDescent="0.25">
-      <c r="Y64" s="18"/>
-      <c r="Z64" s="18"/>
-    </row>
-    <row r="65" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y65" s="18"/>
-      <c r="Z65" s="18"/>
-    </row>
-    <row r="66" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y66" s="18"/>
-      <c r="Z66" s="18"/>
-    </row>
-    <row r="67" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y67" s="18"/>
-      <c r="Z67" s="18"/>
-    </row>
-    <row r="68" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y68" s="18"/>
-      <c r="Z68" s="18"/>
-    </row>
-    <row r="69" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y69" s="18"/>
-      <c r="Z69" s="18"/>
-    </row>
-    <row r="70" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y70" s="18"/>
-      <c r="Z70" s="18"/>
-    </row>
-    <row r="71" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y71" s="18"/>
-      <c r="Z71" s="18"/>
-    </row>
-    <row r="72" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y72" s="18"/>
-      <c r="Z72" s="18"/>
-    </row>
-    <row r="73" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y73" s="18"/>
-      <c r="Z73" s="18"/>
-    </row>
-    <row r="74" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y74" s="18"/>
-      <c r="Z74" s="18"/>
-    </row>
-    <row r="75" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y75" s="18"/>
-      <c r="Z75" s="18"/>
-    </row>
-    <row r="76" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y76" s="18"/>
-      <c r="Z76" s="18"/>
-    </row>
-    <row r="77" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y77" s="18"/>
-      <c r="Z77" s="18"/>
-    </row>
-    <row r="78" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y78" s="18"/>
-      <c r="Z78" s="18"/>
-    </row>
-    <row r="79" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y79" s="18"/>
-      <c r="Z79" s="18"/>
-    </row>
-    <row r="80" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y80" s="18"/>
-      <c r="Z80" s="18"/>
-    </row>
-    <row r="81" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y81" s="18"/>
-      <c r="Z81" s="18"/>
-    </row>
-    <row r="82" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y82" s="18"/>
-      <c r="Z82" s="18"/>
-    </row>
-    <row r="83" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y83" s="18"/>
-      <c r="Z83" s="18"/>
-    </row>
-    <row r="84" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y84" s="18"/>
-      <c r="Z84" s="18"/>
-    </row>
-    <row r="85" spans="25:26" x14ac:dyDescent="0.25">
-      <c r="Y85" s="18"/>
-      <c r="Z85" s="18"/>
+    </row>
+    <row r="55" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>48</v>
+      </c>
+      <c r="G55">
+        <f>(1.602*(10^(-19)))*1000</f>
+        <v>1.6019999999999999E-16</v>
+      </c>
+      <c r="H55" t="s">
+        <v>52</v>
+      </c>
+      <c r="J55" t="s">
+        <v>48</v>
+      </c>
+      <c r="K55">
+        <f>1.602*(10^(-19))</f>
+        <v>1.602E-19</v>
+      </c>
+      <c r="L55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>49</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56" t="s">
+        <v>10</v>
+      </c>
+      <c r="J56" t="s">
+        <v>49</v>
+      </c>
+      <c r="K56">
+        <f>1/1000</f>
+        <v>1E-3</v>
+      </c>
+      <c r="L56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="U57" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="V57" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="W57" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="U58" s="16">
+        <v>0.36030000000000001</v>
+      </c>
+      <c r="V58" s="16">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="W58" s="16">
+        <v>0.72060000000000002</v>
+      </c>
+      <c r="AA58">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="59" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>24</v>
+      </c>
+      <c r="G59">
+        <f>(G53*G52)/(G55*G56*G54)</f>
+        <v>1046178310631264.1</v>
+      </c>
+      <c r="J59" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="K59" s="16">
+        <f>ROUND((K53*K52)/(K55*K56*K54),4)</f>
+        <v>1.04617831063126E+18</v>
+      </c>
+      <c r="L59" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="S59" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="R60" t="s">
+        <v>59</v>
+      </c>
+      <c r="S60" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="T60" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U60" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="R61">
+        <f>S61*0.02</f>
+        <v>0</v>
+      </c>
+      <c r="S61" s="9">
+        <v>0</v>
+      </c>
+      <c r="T61" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="U61" s="15">
+        <f>T61*$AA$58</f>
+        <v>1.0000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="R62">
+        <f t="shared" ref="R62:R81" si="5">S62*0.02</f>
+        <v>0.2</v>
+      </c>
+      <c r="S62" s="9">
+        <v>10</v>
+      </c>
+      <c r="T62">
+        <v>2.1</v>
+      </c>
+      <c r="U62" s="15">
+        <f t="shared" ref="U62:U81" si="6">T62*$AA$58</f>
+        <v>0.10500000000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="R63">
+        <f t="shared" si="5"/>
+        <v>0.4</v>
+      </c>
+      <c r="S63" s="9">
+        <v>20</v>
+      </c>
+      <c r="T63" s="4">
+        <v>4</v>
+      </c>
+      <c r="U63" s="15">
+        <f t="shared" si="6"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="64" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="R64">
+        <f t="shared" si="5"/>
+        <v>0.6</v>
+      </c>
+      <c r="S64" s="9">
+        <v>30</v>
+      </c>
+      <c r="T64" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="U64" s="15">
+        <f t="shared" si="6"/>
+        <v>0.29500000000000004</v>
+      </c>
+    </row>
+    <row r="65" spans="18:21" x14ac:dyDescent="0.25">
+      <c r="R65">
+        <f t="shared" si="5"/>
+        <v>0.8</v>
+      </c>
+      <c r="S65" s="9">
+        <v>40</v>
+      </c>
+      <c r="T65" s="4">
+        <v>7.8</v>
+      </c>
+      <c r="U65" s="15">
+        <f t="shared" si="6"/>
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="66" spans="18:21" x14ac:dyDescent="0.25">
+      <c r="R66">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="S66" s="9">
+        <v>50</v>
+      </c>
+      <c r="T66" s="4">
+        <v>9.6</v>
+      </c>
+      <c r="U66" s="15">
+        <f t="shared" si="6"/>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="67" spans="18:21" x14ac:dyDescent="0.25">
+      <c r="R67">
+        <f t="shared" si="5"/>
+        <v>1.2</v>
+      </c>
+      <c r="S67" s="9">
+        <v>60</v>
+      </c>
+      <c r="T67" s="4">
+        <v>11.5</v>
+      </c>
+      <c r="U67" s="15">
+        <f t="shared" si="6"/>
+        <v>0.57500000000000007</v>
+      </c>
+    </row>
+    <row r="68" spans="18:21" x14ac:dyDescent="0.25">
+      <c r="R68">
+        <f t="shared" si="5"/>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="S68" s="9">
+        <v>70</v>
+      </c>
+      <c r="T68" s="4">
+        <v>13.4</v>
+      </c>
+      <c r="U68" s="15">
+        <f t="shared" si="6"/>
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="69" spans="18:21" x14ac:dyDescent="0.25">
+      <c r="R69">
+        <f t="shared" si="5"/>
+        <v>1.6</v>
+      </c>
+      <c r="S69" s="9">
+        <v>80</v>
+      </c>
+      <c r="T69" s="4">
+        <v>15.1</v>
+      </c>
+      <c r="U69" s="15">
+        <f t="shared" si="6"/>
+        <v>0.755</v>
+      </c>
+    </row>
+    <row r="70" spans="18:21" x14ac:dyDescent="0.25">
+      <c r="R70">
+        <f t="shared" si="5"/>
+        <v>1.8</v>
+      </c>
+      <c r="S70" s="9">
+        <v>90</v>
+      </c>
+      <c r="T70" s="4">
+        <v>17</v>
+      </c>
+      <c r="U70" s="15">
+        <f t="shared" si="6"/>
+        <v>0.85000000000000009</v>
+      </c>
+    </row>
+    <row r="71" spans="18:21" x14ac:dyDescent="0.25">
+      <c r="R71">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="S71" s="9">
+        <v>100</v>
+      </c>
+      <c r="T71" s="4">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="U71" s="15">
+        <f t="shared" si="6"/>
+        <v>0.93000000000000016</v>
+      </c>
+    </row>
+    <row r="72" spans="18:21" x14ac:dyDescent="0.25">
+      <c r="R72">
+        <f t="shared" si="5"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S72" s="9">
+        <v>110</v>
+      </c>
+      <c r="T72" s="4">
+        <v>20.5</v>
+      </c>
+      <c r="U72" s="15">
+        <f t="shared" si="6"/>
+        <v>1.0250000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="18:21" x14ac:dyDescent="0.25">
+      <c r="R73">
+        <f t="shared" si="5"/>
+        <v>2.4</v>
+      </c>
+      <c r="S73" s="9">
+        <v>120</v>
+      </c>
+      <c r="T73" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="U73" s="15">
+        <f t="shared" si="6"/>
+        <v>1.115</v>
+      </c>
+    </row>
+    <row r="74" spans="18:21" x14ac:dyDescent="0.25">
+      <c r="R74">
+        <f t="shared" si="5"/>
+        <v>2.6</v>
+      </c>
+      <c r="S74" s="9">
+        <v>130</v>
+      </c>
+      <c r="T74" s="4">
+        <v>24</v>
+      </c>
+      <c r="U74" s="15">
+        <f t="shared" si="6"/>
+        <v>1.2000000000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="18:21" x14ac:dyDescent="0.25">
+      <c r="R75">
+        <f t="shared" si="5"/>
+        <v>2.8000000000000003</v>
+      </c>
+      <c r="S75" s="9">
+        <v>140</v>
+      </c>
+      <c r="T75" s="4">
+        <v>25.8</v>
+      </c>
+      <c r="U75" s="15">
+        <f t="shared" si="6"/>
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="76" spans="18:21" x14ac:dyDescent="0.25">
+      <c r="R76">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="S76" s="9">
+        <v>150</v>
+      </c>
+      <c r="T76" s="4">
+        <v>27.6</v>
+      </c>
+      <c r="U76" s="15">
+        <f t="shared" si="6"/>
+        <v>1.3800000000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="18:21" x14ac:dyDescent="0.25">
+      <c r="R77">
+        <f t="shared" si="5"/>
+        <v>3.2</v>
+      </c>
+      <c r="S77" s="9">
+        <v>160</v>
+      </c>
+      <c r="T77" s="4">
+        <v>29.3</v>
+      </c>
+      <c r="U77" s="15">
+        <f t="shared" si="6"/>
+        <v>1.4650000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="18:21" x14ac:dyDescent="0.25">
+      <c r="R78">
+        <f t="shared" si="5"/>
+        <v>3.4</v>
+      </c>
+      <c r="S78" s="9">
+        <v>170</v>
+      </c>
+      <c r="T78" s="4">
+        <v>31</v>
+      </c>
+      <c r="U78" s="15">
+        <f t="shared" si="6"/>
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="79" spans="18:21" x14ac:dyDescent="0.25">
+      <c r="R79">
+        <f t="shared" si="5"/>
+        <v>3.6</v>
+      </c>
+      <c r="S79" s="9">
+        <v>180</v>
+      </c>
+      <c r="T79" s="4">
+        <v>32.6</v>
+      </c>
+      <c r="U79" s="15">
+        <f t="shared" si="6"/>
+        <v>1.6300000000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="18:21" x14ac:dyDescent="0.25">
+      <c r="R80">
+        <f t="shared" si="5"/>
+        <v>3.8000000000000003</v>
+      </c>
+      <c r="S80" s="9">
+        <v>190</v>
+      </c>
+      <c r="T80" s="4">
+        <v>34.4</v>
+      </c>
+      <c r="U80" s="15">
+        <f t="shared" si="6"/>
+        <v>1.72</v>
+      </c>
+    </row>
+    <row r="81" spans="18:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R81">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="S81" s="11">
+        <v>200</v>
+      </c>
+      <c r="T81" s="12">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="U81" s="15">
+        <f t="shared" si="6"/>
+        <v>1.79</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Skonczono ostatnie laby z Halla Fiz2
</commit_message>
<xml_diff>
--- a/FIZ2/Halla.xlsx
+++ b/FIZ2/Halla.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kamil\Desktop\Stary Folder\studia_git\FIZ2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kamil\Desktop\Stary Folder\studia\Semestr3\studia_git\FIZ2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93350134-B612-4289-8627-4571814B01AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533FE9C7-7D2B-4315-B8DB-285A1A0905FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22106E2D-535D-4D61-8847-61EECC787C3F}"/>
   </bookViews>
@@ -297,10 +297,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -548,10 +549,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1889,8 +1890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A447AA0A-D447-4B02-AC14-94CF8529AAB0}">
   <dimension ref="C4:DD81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U45" sqref="U45"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y51" sqref="Y51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1902,7 +1903,8 @@
     <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.140625" customWidth="1"/>
     <col min="24" max="24" width="8.85546875" customWidth="1"/>
-    <col min="25" max="26" width="5" customWidth="1"/>
+    <col min="25" max="25" width="8" customWidth="1"/>
+    <col min="26" max="26" width="5" customWidth="1"/>
     <col min="27" max="29" width="10.7109375" customWidth="1"/>
     <col min="30" max="108" width="5" customWidth="1"/>
   </cols>
@@ -2937,7 +2939,7 @@
       <c r="W13" t="s">
         <v>80</v>
       </c>
-      <c r="X13">
+      <c r="X13" s="15">
         <f>ROUND(V13/SQRT(3),1)</f>
         <v>0.1</v>
       </c>
@@ -3657,8 +3659,8 @@
         <v>2.36436298202665E+16</v>
       </c>
       <c r="W25" s="16">
-        <f>2*U25</f>
-        <v>4.5199999999999997E-2</v>
+        <f>2*V25</f>
+        <v>4.7287259640533E+16</v>
       </c>
     </row>
     <row r="26" spans="3:29" x14ac:dyDescent="0.25">
@@ -4311,8 +4313,8 @@
         <v>4.2309000000000001</v>
       </c>
       <c r="W44" s="16">
-        <f>2*U44</f>
-        <v>3.1199999999999999E-2</v>
+        <f>2*V44</f>
+        <v>8.4618000000000002</v>
       </c>
     </row>
     <row r="45" spans="5:29" x14ac:dyDescent="0.25">
@@ -4396,6 +4398,18 @@
       <c r="Q48" s="4">
         <v>25.8</v>
       </c>
+      <c r="W48" s="22">
+        <f>0.1/35.8</f>
+        <v>2.7932960893854754E-3</v>
+      </c>
+      <c r="X48">
+        <f>2.309/200</f>
+        <v>1.1545000000000001E-2</v>
+      </c>
+      <c r="Y48">
+        <f>0.5774/30</f>
+        <v>1.9246666666666669E-2</v>
+      </c>
     </row>
     <row r="49" spans="6:27" x14ac:dyDescent="0.25">
       <c r="O49" s="9">
@@ -4420,6 +4434,22 @@
       <c r="Q50" s="4">
         <v>29.3</v>
       </c>
+      <c r="T50">
+        <f>H40*H40</f>
+        <v>3.5880100000000004E-3</v>
+      </c>
+      <c r="W50">
+        <f>V20/H28</f>
+        <v>1.0064245810055867E-2</v>
+      </c>
+      <c r="X50">
+        <f>X14/I28</f>
+        <v>3.0075187969924809E-3</v>
+      </c>
+      <c r="Y50">
+        <f>V19/G28</f>
+        <v>1.1547E-2</v>
+      </c>
     </row>
     <row r="51" spans="6:27" x14ac:dyDescent="0.25">
       <c r="F51" t="s">
@@ -4435,6 +4465,10 @@
       <c r="Q51" s="4">
         <v>31</v>
       </c>
+      <c r="T51">
+        <f>G40*G40*G28*G28</f>
+        <v>9.9999999999999985E-3</v>
+      </c>
     </row>
     <row r="52" spans="6:27" x14ac:dyDescent="0.25">
       <c r="F52" t="s">
@@ -4632,7 +4666,7 @@
       <c r="T60" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="U60" s="22" t="s">
+      <c r="U60" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>